<commit_message>
Correcoes na Planilha de Questoes
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwecko/Scripts/Assymble_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40167EC0-016D-314B-B1C3-BFCC7834F11A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514C244F-8176-154E-9363-F3E4E21F82D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4180" yWindow="5060" windowWidth="27560" windowHeight="14960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4180" yWindow="5060" windowWidth="27560" windowHeight="14960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="questoes" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="38">
   <si>
     <t>TIPO</t>
   </si>
@@ -552,7 +552,7 @@
   </sheetPr>
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -883,8 +883,8 @@
   </sheetPr>
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:M5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1052,23 +1052,45 @@
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
     </row>
-    <row r="6" spans="1:14" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+    <row r="6" spans="1:14" s="1" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="L6" s="2"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
     </row>
-    <row r="7" spans="1:14" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>

</xml_diff>